<commit_message>
:+1: Dataset For the Temperature Project is completed
</commit_message>
<xml_diff>
--- a/Datasets/HRProject_dummydata.xlsx
+++ b/Datasets/HRProject_dummydata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Files\Nesternship-HR-Project-Medical-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Files\Nesternship-HR-Project-Medical-Data\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF6852ED-D237-4DA3-BCEF-9A59369E5099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0460ABCA-4781-46B3-A438-2D1BAD75AA20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
   <si>
     <t xml:space="preserve">Personal Infromation </t>
   </si>
@@ -169,9 +160,6 @@
     <t xml:space="preserve">Temperature </t>
   </si>
   <si>
-    <t>Samin Alam</t>
-  </si>
-  <si>
     <t>HR</t>
   </si>
   <si>
@@ -230,12 +218,30 @@
   </si>
   <si>
     <t>Child 2</t>
+  </si>
+  <si>
+    <t>Rabab Shayra</t>
+  </si>
+  <si>
+    <t>Sumaiya Akhtar</t>
+  </si>
+  <si>
+    <t>Arif Ahmed Nowfel</t>
+  </si>
+  <si>
+    <t>Ayesha Mou</t>
+  </si>
+  <si>
+    <t>Mazharul Islam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -313,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -523,24 +529,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -561,8 +554,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -618,6 +609,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,58 +930,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="28" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="28" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="28" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="28" t="s">
+      <c r="P1" s="28"/>
+      <c r="Q1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="30"/>
-      <c r="S1" s="28" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="28" t="s">
+      <c r="T1" s="28"/>
+      <c r="U1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="28" t="s">
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="28" t="s">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="30"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="28"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -1227,18 +1222,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECF6690-A3BF-4335-B655-AAC0CB4E8EC5}">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.54296875" customWidth="1"/>
     <col min="8" max="8" width="8.54296875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
@@ -1246,36 +1242,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="31" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
@@ -1309,60 +1305,60 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="16">
-        <v>11034485</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="19">
-        <v>44120</v>
-      </c>
-      <c r="F4" s="20">
-        <v>0.3576388888888889</v>
+      <c r="B4">
+        <v>88456287</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="23">
+        <v>44100</v>
+      </c>
+      <c r="F4" s="43">
+        <v>0.34791666666666665</v>
       </c>
       <c r="G4">
+        <v>37.4</v>
+      </c>
+      <c r="H4" s="23">
+        <v>44100</v>
+      </c>
+      <c r="I4" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J4">
         <v>36.5</v>
       </c>
-      <c r="H4" s="19">
-        <v>44120</v>
-      </c>
-      <c r="I4" s="20">
-        <v>0.73611111111111116</v>
-      </c>
-      <c r="J4" s="21">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1372,101 +1368,1308 @@
         <v>97352991</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="25">
+        <v>29</v>
+      </c>
+      <c r="E5" s="23">
         <v>44100</v>
+      </c>
+      <c r="F5" s="43">
+        <v>0.34930555555555554</v>
       </c>
       <c r="G5">
         <v>36.799999999999997</v>
       </c>
+      <c r="H5" s="23">
+        <v>44100</v>
+      </c>
+      <c r="I5" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J5">
+        <v>37.200000000000003</v>
+      </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E6" s="25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>28748821</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="23">
         <v>44100</v>
+      </c>
+      <c r="F6" s="43">
+        <v>0.34930555555555554</v>
       </c>
       <c r="G6">
         <v>37.5</v>
       </c>
+      <c r="H6" s="23">
+        <v>44100</v>
+      </c>
+      <c r="I6" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J6">
+        <v>36.4</v>
+      </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E7" s="25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>94872843</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="23">
         <v>44100</v>
+      </c>
+      <c r="F7" s="43">
+        <v>0.3527777777777778</v>
       </c>
       <c r="G7">
         <v>36.1</v>
       </c>
+      <c r="H7" s="23">
+        <v>44100</v>
+      </c>
+      <c r="I7" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J7">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E8" s="25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>66387726</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="23">
         <v>44100</v>
       </c>
+      <c r="F8" s="43">
+        <v>0.35347222222222219</v>
+      </c>
       <c r="G8">
-        <v>37.4</v>
+        <v>36.9</v>
+      </c>
+      <c r="H8" s="23">
+        <v>44100</v>
+      </c>
+      <c r="I8" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J8">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E9" s="25">
+      <c r="A9" s="41">
+        <v>6</v>
+      </c>
+      <c r="B9" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="42">
         <v>44100</v>
       </c>
-      <c r="G9">
-        <v>36.9</v>
+      <c r="F9" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G9" s="41">
+        <v>36.5</v>
+      </c>
+      <c r="H9" s="42">
+        <v>44100</v>
+      </c>
+      <c r="I9" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J9" s="41">
+        <v>36.1</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E10" s="25">
-        <v>44100</v>
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>88456287</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="23">
+        <v>44101</v>
+      </c>
+      <c r="F10" s="43">
+        <v>0.34791666666666665</v>
       </c>
       <c r="G10">
         <v>36.200000000000003</v>
       </c>
+      <c r="H10" s="23">
+        <v>44101</v>
+      </c>
+      <c r="I10" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J10">
+        <v>37.4</v>
+      </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E11" s="25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>97352991</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="23">
         <v>44101</v>
+      </c>
+      <c r="F11" s="43">
+        <v>0.34930555555555554</v>
       </c>
       <c r="G11">
         <v>36.9</v>
       </c>
+      <c r="H11" s="23">
+        <v>44101</v>
+      </c>
+      <c r="I11" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J11">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E12" s="25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>28748821</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="23">
         <v>44101</v>
+      </c>
+      <c r="F12" s="43">
+        <v>0.34930555555555554</v>
       </c>
       <c r="G12">
         <v>36.1</v>
       </c>
+      <c r="H12" s="23">
+        <v>44101</v>
+      </c>
+      <c r="I12" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J12">
+        <v>37.9</v>
+      </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E13" s="25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>94872843</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="23">
         <v>44101</v>
+      </c>
+      <c r="F13" s="43">
+        <v>0.3527777777777778</v>
       </c>
       <c r="G13">
         <v>36.200000000000003</v>
       </c>
+      <c r="H13" s="23">
+        <v>44101</v>
+      </c>
+      <c r="I13" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J13">
+        <v>37.200000000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E14" s="25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>66387726</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="23">
         <v>44101</v>
+      </c>
+      <c r="F14" s="43">
+        <v>0.35347222222222219</v>
       </c>
       <c r="G14">
         <v>36.799999999999997</v>
       </c>
+      <c r="H14" s="23">
+        <v>44101</v>
+      </c>
+      <c r="I14" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J14">
+        <v>36.1</v>
+      </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E15" s="25">
+      <c r="A15" s="41">
+        <v>12</v>
+      </c>
+      <c r="B15" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="42">
         <v>44101</v>
       </c>
-      <c r="G15">
+      <c r="F15" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G15" s="41">
         <v>36.4</v>
       </c>
+      <c r="H15" s="42">
+        <v>44101</v>
+      </c>
+      <c r="I15" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J15" s="41">
+        <v>36.4</v>
+      </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="E16" s="25">
-        <v>44101</v>
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>88456287</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="23">
+        <v>44102</v>
+      </c>
+      <c r="F16" s="43">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="G16">
+        <v>36.6</v>
+      </c>
+      <c r="H16" s="23">
+        <v>44102</v>
+      </c>
+      <c r="I16" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J16">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>97352991</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="23">
+        <v>44102</v>
+      </c>
+      <c r="F17" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G17">
+        <v>36.9</v>
+      </c>
+      <c r="H17" s="23">
+        <v>44102</v>
+      </c>
+      <c r="I17" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J17">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>28748821</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="23">
+        <v>44102</v>
+      </c>
+      <c r="F18" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G18">
+        <v>36.9</v>
+      </c>
+      <c r="H18" s="23">
+        <v>44102</v>
+      </c>
+      <c r="I18" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J18">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>94872843</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="23">
+        <v>44102</v>
+      </c>
+      <c r="F19" s="43">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="G19">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="H19" s="23">
+        <v>44102</v>
+      </c>
+      <c r="I19" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>66387726</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="23">
+        <v>44102</v>
+      </c>
+      <c r="F20" s="43">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="G20">
+        <v>36.9</v>
+      </c>
+      <c r="H20" s="23">
+        <v>44102</v>
+      </c>
+      <c r="I20" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J20">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="41">
+        <v>18</v>
+      </c>
+      <c r="B21" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="42">
+        <v>44102</v>
+      </c>
+      <c r="F21" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G21" s="41">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="H21" s="42">
+        <v>44102</v>
+      </c>
+      <c r="I21" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J21" s="41">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>88456287</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="23">
+        <v>44103</v>
+      </c>
+      <c r="F22" s="43">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="G22">
+        <v>37.1</v>
+      </c>
+      <c r="H22" s="23">
+        <v>44103</v>
+      </c>
+      <c r="I22" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J22">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>97352991</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="23">
+        <v>44103</v>
+      </c>
+      <c r="F23" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G23">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H23" s="23">
+        <v>44103</v>
+      </c>
+      <c r="I23" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J23">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>28748821</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="23">
+        <v>44103</v>
+      </c>
+      <c r="F24" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G24">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="H24" s="23">
+        <v>44103</v>
+      </c>
+      <c r="I24" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J24">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>94872843</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="23">
+        <v>44103</v>
+      </c>
+      <c r="F25" s="43">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="G25">
+        <v>37.4</v>
+      </c>
+      <c r="H25" s="23">
+        <v>44103</v>
+      </c>
+      <c r="I25" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J25">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>66387726</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="23">
+        <v>44103</v>
+      </c>
+      <c r="F26" s="43">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="G26">
+        <v>37.6</v>
+      </c>
+      <c r="H26" s="23">
+        <v>44103</v>
+      </c>
+      <c r="I26" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J26">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="41">
+        <v>24</v>
+      </c>
+      <c r="B27" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="42">
+        <v>44103</v>
+      </c>
+      <c r="F27" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G27" s="41">
+        <v>36.9</v>
+      </c>
+      <c r="H27" s="42">
+        <v>44103</v>
+      </c>
+      <c r="I27" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J27" s="41">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>88456287</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="23">
+        <v>44104</v>
+      </c>
+      <c r="F28" s="43">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="G28">
+        <v>37.9</v>
+      </c>
+      <c r="H28" s="23">
+        <v>44104</v>
+      </c>
+      <c r="I28" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J28">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>97352991</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="23">
+        <v>44104</v>
+      </c>
+      <c r="F29" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G29">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H29" s="23">
+        <v>44104</v>
+      </c>
+      <c r="I29" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J29">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>28748821</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="23">
+        <v>44104</v>
+      </c>
+      <c r="F30" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G30">
+        <v>36.4</v>
+      </c>
+      <c r="H30" s="23">
+        <v>44104</v>
+      </c>
+      <c r="I30" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J30">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>94872843</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="23">
+        <v>44104</v>
+      </c>
+      <c r="F31" s="43">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="G31">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H31" s="23">
+        <v>44104</v>
+      </c>
+      <c r="I31" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J31">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>66387726</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="23">
+        <v>44104</v>
+      </c>
+      <c r="F32" s="43">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="G32">
+        <v>36.5</v>
+      </c>
+      <c r="H32" s="23">
+        <v>44104</v>
+      </c>
+      <c r="I32" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J32">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="41">
+        <v>30</v>
+      </c>
+      <c r="B33" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="42">
+        <v>44104</v>
+      </c>
+      <c r="F33" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G33" s="41">
+        <v>36.4</v>
+      </c>
+      <c r="H33" s="42">
+        <v>44104</v>
+      </c>
+      <c r="I33" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J33" s="41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>88456287</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="23">
+        <v>44105</v>
+      </c>
+      <c r="F34" s="43">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="G34">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="H34" s="23">
+        <v>44105</v>
+      </c>
+      <c r="I34" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J34">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>97352991</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="23">
+        <v>44105</v>
+      </c>
+      <c r="F35" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G35">
+        <v>36.9</v>
+      </c>
+      <c r="H35" s="23">
+        <v>44105</v>
+      </c>
+      <c r="I35" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J35">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>28748821</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="23">
+        <v>44105</v>
+      </c>
+      <c r="F36" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G36">
+        <v>37.5</v>
+      </c>
+      <c r="H36" s="23">
+        <v>44105</v>
+      </c>
+      <c r="I36" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J36">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>94872843</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="23">
+        <v>44105</v>
+      </c>
+      <c r="F37" s="43">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="G37">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="H37" s="23">
+        <v>44105</v>
+      </c>
+      <c r="I37" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J37">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>66387726</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="23">
+        <v>44105</v>
+      </c>
+      <c r="F38" s="43">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="G38">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="H38" s="23">
+        <v>44105</v>
+      </c>
+      <c r="I38" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J38">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="41">
+        <v>36</v>
+      </c>
+      <c r="B39" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="42">
+        <v>44105</v>
+      </c>
+      <c r="F39" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G39" s="41">
+        <v>37.5</v>
+      </c>
+      <c r="H39" s="42">
+        <v>44105</v>
+      </c>
+      <c r="I39" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J39" s="41">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>88456287</v>
+      </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="23">
+        <v>44106</v>
+      </c>
+      <c r="F40" s="43">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="G40">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H40" s="23">
+        <v>44106</v>
+      </c>
+      <c r="I40" s="43">
+        <v>0.22291666666666665</v>
+      </c>
+      <c r="J40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>97352991</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="23">
+        <v>44106</v>
+      </c>
+      <c r="F41" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G41">
+        <v>36.4</v>
+      </c>
+      <c r="H41" s="23">
+        <v>44106</v>
+      </c>
+      <c r="I41" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>28748821</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="23">
+        <v>44106</v>
+      </c>
+      <c r="F42" s="43">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="G42">
+        <v>37.5</v>
+      </c>
+      <c r="H42" s="23">
+        <v>44106</v>
+      </c>
+      <c r="I42" s="43">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="J42">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>94872843</v>
+      </c>
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="23">
+        <v>44106</v>
+      </c>
+      <c r="F43" s="43">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="G43">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="H43" s="23">
+        <v>44106</v>
+      </c>
+      <c r="I43" s="43">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="J43">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>66387726</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="23">
+        <v>44106</v>
+      </c>
+      <c r="F44" s="43">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="G44">
+        <v>37.9</v>
+      </c>
+      <c r="H44" s="23">
+        <v>44106</v>
+      </c>
+      <c r="I44" s="43">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="J44">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="41">
+        <v>42</v>
+      </c>
+      <c r="B45" s="41">
+        <v>11034485</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="42">
+        <v>44106</v>
+      </c>
+      <c r="F45" s="44">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="G45" s="41">
+        <v>37.1</v>
+      </c>
+      <c r="H45" s="42">
+        <v>44106</v>
+      </c>
+      <c r="I45" s="44">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="J45" s="41">
+        <v>37.700000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +2683,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{73984CA4-CA83-496A-9A82-EB412FF9032F}">
           <x14:formula1>
             <xm:f>'drop down'!$G$2:$G$3</xm:f>
@@ -1522,16 +2725,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
@@ -1540,10 +2743,10 @@
         <v>13</v>
       </c>
       <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
         <v>49</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1553,7 +2756,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1584,19 +2787,19 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -1606,10 +2809,10 @@
         <v>3515012</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
@@ -1651,16 +2854,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
         <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1674,37 +2877,37 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
         <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>